<commit_message>
Fix: Remove hardcoded 7-month limit to properly include all historical data
- Fixed bug in analyze_category() that was hardcoded to only use first 7 months
- System now dynamically uses all available months with data
- Added automatic next-month detection based on last month with data
- Enhanced web UI to clearly display target forecast month and data range
- September 2025 forecast now correctly includes August actuals
- Forecast accuracy improved: $92,228.53 → $90,456.98 with August data

Key changes:
* Dynamic month detection in load_data()
* Removed [:7] hardcoded limit in historical data processing
* Updated web interface with clear month labels and data range display
* All forecasts now properly reflect complete historical dataset
</commit_message>
<xml_diff>
--- a/Input/Actual.xlsx
+++ b/Input/Actual.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Accurals\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C940D00-FC42-4AB7-A5FD-D4BA189AD3B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40231A12-D808-4C72-9D41-45A64DCE4613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{AF23E715-82B4-40CB-A084-D8B9ACEC0240}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AF23E715-82B4-40CB-A084-D8B9ACEC0240}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -615,6 +615,9 @@
       <c r="J2">
         <v>12467.895905999998</v>
       </c>
+      <c r="K2">
+        <v>9234.4775200000004</v>
+      </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -647,6 +650,9 @@
       <c r="J3">
         <v>36538.81560400001</v>
       </c>
+      <c r="K3">
+        <v>32092.500000000004</v>
+      </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -679,6 +685,9 @@
       <c r="J4">
         <v>17387.349999999999</v>
       </c>
+      <c r="K4">
+        <v>14196.32</v>
+      </c>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -711,6 +720,9 @@
       <c r="J5">
         <v>31348.396500000003</v>
       </c>
+      <c r="K5">
+        <v>25595.16</v>
+      </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -742,6 +754,9 @@
       </c>
       <c r="J6">
         <v>7937.5360049999999</v>
+      </c>
+      <c r="K6">
+        <v>5004.93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>